<commit_message>
Remove unused training images and masks to clean up the dataset
</commit_message>
<xml_diff>
--- a/results/UNet_Berechnen.xlsx
+++ b/results/UNet_Berechnen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Masterarbeit\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8796CBDF-DFD1-4B72-9CBD-4E7AD3A3FEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28ED9A81-F79E-47C9-8827-CAAD37959846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28935" yWindow="0" windowWidth="14025" windowHeight="15585" xr2:uid="{3538B6B0-B1DE-42DE-A4BF-20A52176B29F}"/>
+    <workbookView xWindow="17265" yWindow="1605" windowWidth="21600" windowHeight="11295" xr2:uid="{3538B6B0-B1DE-42DE-A4BF-20A52176B29F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Stridehöhe</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>ConvTranspose</t>
+  </si>
+  <si>
+    <t>Maxpool</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Dimension</t>
   </si>
 </sst>
 </file>
@@ -428,37 +437,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14B8341-8BAF-45F6-AAC9-F238FA0AA158}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>622</v>
+        <v>188</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -471,8 +489,14 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -483,10 +507,17 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <f>I2/I3</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -497,51 +528,95 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <f>I4</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <f>B3*(B2-1)+B4-2*B5</f>
-        <v>1242</v>
+        <v>374</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
       <c r="F7">
         <f>(F2+2*F5-F4)/(F3)+1</f>
-        <v>374</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <f>I6/I7</f>
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10">
         <f>F7</f>
-        <v>374</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <f>I8</f>
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>0</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>2</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <f>I10/I11</f>
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>3</v>
       </c>
@@ -549,13 +624,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <f>I12</f>
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>4</v>
       </c>
       <c r="F15">
         <f>(F10+2*F13-F12)/(F11)+1</f>
-        <v>374</v>
+        <v>50</v>
+      </c>
+      <c r="H15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16">
+        <f>I14/I15</f>
+        <v>5.875</v>
       </c>
     </row>
   </sheetData>
@@ -564,20 +663,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="768ccc40-3631-450f-87b0-3142498a2bc0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="768ccc40-3631-450f-87b0-3142498a2bc0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -808,6 +907,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A19DE826-1672-41B5-8418-839BC21FE4A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{151798C9-BF44-400C-90BF-D6075FFBD701}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -820,14 +927,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="4bbe938f-0039-42e7-aafe-6bba795bd972"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A19DE826-1672-41B5-8418-839BC21FE4A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>